<commit_message>
Week 8b display bash file
</commit_message>
<xml_diff>
--- a/Index_of_functions_formatted.xlsx
+++ b/Index_of_functions_formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Helene/Desktop/R_Github/DGS_LG_Labs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7734AB-5C62-EA49-B840-3053680B2C18}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0D3CD3-FE76-0149-A34E-E0A0CA2510CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="386">
   <si>
     <t>W0</t>
   </si>
@@ -1168,9 +1168,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Index of Funtions</t>
-  </si>
-  <si>
     <t>Week2_vignette</t>
   </si>
   <si>
@@ -1178,6 +1175,12 @@
   </si>
   <si>
     <t>Key to files:</t>
+  </si>
+  <si>
+    <t>Index of Functions</t>
+  </si>
+  <si>
+    <t>readLines</t>
   </si>
 </sst>
 </file>
@@ -2079,10 +2082,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R370"/>
+  <dimension ref="A1:R371"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
+      <selection activeCell="A279" sqref="A279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -2094,18 +2097,18 @@
   <sheetData>
     <row r="1" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -2113,7 +2116,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:18" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -9210,7 +9213,7 @@
     </row>
     <row r="279" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A279" s="4" t="s">
-        <v>288</v>
+        <v>385</v>
       </c>
       <c r="B279" s="5"/>
       <c r="C279" s="5"/>
@@ -9222,10 +9225,10 @@
       <c r="I279" s="5"/>
       <c r="J279" s="5"/>
       <c r="K279" s="5"/>
-      <c r="L279" s="5"/>
-      <c r="M279" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="L279" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="M279" s="5"/>
       <c r="N279" s="5"/>
       <c r="O279" s="5"/>
       <c r="P279" s="5"/>
@@ -9234,7 +9237,7 @@
     </row>
     <row r="280" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A280" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B280" s="5"/>
       <c r="C280" s="5"/>
@@ -9246,10 +9249,10 @@
       <c r="I280" s="5"/>
       <c r="J280" s="5"/>
       <c r="K280" s="5"/>
-      <c r="L280" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="M280" s="5"/>
+      <c r="L280" s="5"/>
+      <c r="M280" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N280" s="5"/>
       <c r="O280" s="5"/>
       <c r="P280" s="5"/>
@@ -9258,7 +9261,7 @@
     </row>
     <row r="281" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A281" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B281" s="5"/>
       <c r="C281" s="5"/>
@@ -9269,67 +9272,67 @@
       <c r="H281" s="5"/>
       <c r="I281" s="5"/>
       <c r="J281" s="5"/>
-      <c r="K281" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="L281" s="5"/>
+      <c r="K281" s="5"/>
+      <c r="L281" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="M281" s="5"/>
       <c r="N281" s="5"/>
       <c r="O281" s="5"/>
-      <c r="P281" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="P281" s="5"/>
       <c r="Q281" s="5"/>
       <c r="R281" s="5"/>
     </row>
     <row r="282" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A282" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="B282" s="5" t="s">
-        <v>380</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="B282" s="5"/>
       <c r="C282" s="5"/>
-      <c r="D282" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="D282" s="5"/>
       <c r="E282" s="5"/>
       <c r="F282" s="5"/>
       <c r="G282" s="5"/>
-      <c r="H282" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="H282" s="5"/>
       <c r="I282" s="5"/>
       <c r="J282" s="5"/>
-      <c r="K282" s="5"/>
+      <c r="K282" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L282" s="5"/>
-      <c r="M282" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M282" s="5"/>
       <c r="N282" s="5"/>
-      <c r="O282" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="P282" s="5"/>
+      <c r="O282" s="5"/>
+      <c r="P282" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q282" s="5"/>
       <c r="R282" s="5"/>
     </row>
     <row r="283" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A283" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="B283" s="5"/>
+        <v>291</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="C283" s="5"/>
-      <c r="D283" s="5"/>
+      <c r="D283" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="E283" s="5"/>
       <c r="F283" s="5"/>
       <c r="G283" s="5"/>
-      <c r="H283" s="5"/>
+      <c r="H283" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="I283" s="5"/>
       <c r="J283" s="5"/>
       <c r="K283" s="5"/>
       <c r="L283" s="5"/>
-      <c r="M283" s="5"/>
+      <c r="M283" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N283" s="5"/>
       <c r="O283" s="5" t="s">
         <v>380</v>
@@ -9340,43 +9343,21 @@
     </row>
     <row r="284" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A284" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B284" s="5"/>
-      <c r="C284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="D284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="E284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="F284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="G284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="H284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="I284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="K284" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="C284" s="5"/>
+      <c r="D284" s="5"/>
+      <c r="E284" s="5"/>
+      <c r="F284" s="5"/>
+      <c r="G284" s="5"/>
+      <c r="H284" s="5"/>
+      <c r="I284" s="5"/>
+      <c r="J284" s="5"/>
+      <c r="K284" s="5"/>
       <c r="L284" s="5"/>
-      <c r="M284" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="N284" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M284" s="5"/>
+      <c r="N284" s="5"/>
       <c r="O284" s="5" t="s">
         <v>380</v>
       </c>
@@ -9386,31 +9367,53 @@
     </row>
     <row r="285" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A285" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B285" s="5"/>
-      <c r="C285" s="5"/>
-      <c r="D285" s="5"/>
-      <c r="E285" s="5"/>
-      <c r="F285" s="5"/>
-      <c r="G285" s="5"/>
-      <c r="H285" s="5"/>
-      <c r="I285" s="5"/>
+      <c r="C285" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D285" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="E285" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="F285" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="G285" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="H285" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="I285" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="J285" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="K285" s="5"/>
+      <c r="K285" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L285" s="5"/>
-      <c r="M285" s="5"/>
-      <c r="N285" s="5"/>
-      <c r="O285" s="5"/>
+      <c r="M285" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="N285" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="O285" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P285" s="5"/>
       <c r="Q285" s="5"/>
       <c r="R285" s="5"/>
     </row>
     <row r="286" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A286" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B286" s="5"/>
       <c r="C286" s="5"/>
@@ -9434,7 +9437,7 @@
     </row>
     <row r="287" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A287" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B287" s="5"/>
       <c r="C287" s="5"/>
@@ -9443,10 +9446,10 @@
       <c r="F287" s="5"/>
       <c r="G287" s="5"/>
       <c r="H287" s="5"/>
-      <c r="I287" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J287" s="5"/>
+      <c r="I287" s="5"/>
+      <c r="J287" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="K287" s="5"/>
       <c r="L287" s="5"/>
       <c r="M287" s="5"/>
@@ -9458,50 +9461,46 @@
     </row>
     <row r="288" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A288" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B288" s="5"/>
       <c r="C288" s="5"/>
       <c r="D288" s="5"/>
       <c r="E288" s="5"/>
       <c r="F288" s="5"/>
-      <c r="G288" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="G288" s="5"/>
       <c r="H288" s="5"/>
-      <c r="I288" s="5"/>
-      <c r="J288" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="I288" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J288" s="5"/>
       <c r="K288" s="5"/>
       <c r="L288" s="5"/>
       <c r="M288" s="5"/>
       <c r="N288" s="5"/>
       <c r="O288" s="5"/>
-      <c r="P288" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="P288" s="5"/>
       <c r="Q288" s="5"/>
       <c r="R288" s="5"/>
     </row>
     <row r="289" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A289" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="B289" s="5" t="s">
-        <v>380</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="B289" s="5"/>
       <c r="C289" s="5"/>
       <c r="D289" s="5"/>
       <c r="E289" s="5"/>
       <c r="F289" s="5"/>
-      <c r="G289" s="5"/>
+      <c r="G289" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="H289" s="5"/>
       <c r="I289" s="5"/>
-      <c r="J289" s="5"/>
-      <c r="K289" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="J289" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="K289" s="5"/>
       <c r="L289" s="5"/>
       <c r="M289" s="5"/>
       <c r="N289" s="5"/>
@@ -9510,41 +9509,47 @@
         <v>380</v>
       </c>
       <c r="Q289" s="5"/>
-      <c r="R289" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R289" s="5"/>
     </row>
     <row r="290" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A290" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="B290" s="5"/>
+        <v>298</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="C290" s="5"/>
-      <c r="D290" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="D290" s="5"/>
       <c r="E290" s="5"/>
       <c r="F290" s="5"/>
       <c r="G290" s="5"/>
       <c r="H290" s="5"/>
       <c r="I290" s="5"/>
       <c r="J290" s="5"/>
-      <c r="K290" s="5"/>
+      <c r="K290" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L290" s="5"/>
       <c r="M290" s="5"/>
       <c r="N290" s="5"/>
       <c r="O290" s="5"/>
-      <c r="P290" s="5"/>
+      <c r="P290" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q290" s="5"/>
-      <c r="R290" s="5"/>
+      <c r="R290" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="291" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A291" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B291" s="5"/>
       <c r="C291" s="5"/>
-      <c r="D291" s="5"/>
+      <c r="D291" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="E291" s="5"/>
       <c r="F291" s="5"/>
       <c r="G291" s="5"/>
@@ -9552,9 +9557,7 @@
       <c r="I291" s="5"/>
       <c r="J291" s="5"/>
       <c r="K291" s="5"/>
-      <c r="L291" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="L291" s="5"/>
       <c r="M291" s="5"/>
       <c r="N291" s="5"/>
       <c r="O291" s="5"/>
@@ -9564,11 +9567,9 @@
     </row>
     <row r="292" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A292" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="B292" s="5" t="s">
-        <v>380</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="B292" s="5"/>
       <c r="C292" s="5"/>
       <c r="D292" s="5"/>
       <c r="E292" s="5"/>
@@ -9581,9 +9582,7 @@
       <c r="L292" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="M292" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M292" s="5"/>
       <c r="N292" s="5"/>
       <c r="O292" s="5"/>
       <c r="P292" s="5"/>
@@ -9592,48 +9591,38 @@
     </row>
     <row r="293" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A293" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="B293" s="5"/>
+        <v>301</v>
+      </c>
+      <c r="B293" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="C293" s="5"/>
       <c r="D293" s="5"/>
       <c r="E293" s="5"/>
-      <c r="F293" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="F293" s="5"/>
       <c r="G293" s="5"/>
-      <c r="H293" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="H293" s="5"/>
       <c r="I293" s="5"/>
-      <c r="J293" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="K293" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="L293" s="5"/>
+      <c r="J293" s="5"/>
+      <c r="K293" s="5"/>
+      <c r="L293" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="M293" s="5" t="s">
         <v>380</v>
       </c>
       <c r="N293" s="5"/>
-      <c r="O293" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="P293" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O293" s="5"/>
+      <c r="P293" s="5"/>
       <c r="Q293" s="5"/>
       <c r="R293" s="5"/>
     </row>
     <row r="294" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A294" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B294" s="5"/>
-      <c r="C294" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="C294" s="5"/>
       <c r="D294" s="5"/>
       <c r="E294" s="5"/>
       <c r="F294" s="5" t="s">
@@ -9643,9 +9632,7 @@
       <c r="H294" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="I294" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="I294" s="5"/>
       <c r="J294" s="5" t="s">
         <v>380</v>
       </c>
@@ -9653,72 +9640,90 @@
         <v>380</v>
       </c>
       <c r="L294" s="5"/>
-      <c r="M294" s="5"/>
+      <c r="M294" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N294" s="5"/>
-      <c r="O294" s="5"/>
-      <c r="P294" s="5"/>
+      <c r="O294" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="P294" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q294" s="5"/>
       <c r="R294" s="5"/>
     </row>
     <row r="295" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A295" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B295" s="5"/>
-      <c r="C295" s="5"/>
+      <c r="C295" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="D295" s="5"/>
       <c r="E295" s="5"/>
-      <c r="F295" s="5"/>
-      <c r="G295" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="H295" s="5"/>
-      <c r="I295" s="5"/>
-      <c r="J295" s="5"/>
+      <c r="F295" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="G295" s="5"/>
+      <c r="H295" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="I295" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J295" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="K295" s="5" t="s">
         <v>380</v>
       </c>
       <c r="L295" s="5"/>
-      <c r="M295" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M295" s="5"/>
       <c r="N295" s="5"/>
-      <c r="O295" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O295" s="5"/>
       <c r="P295" s="5"/>
       <c r="Q295" s="5"/>
       <c r="R295" s="5"/>
     </row>
     <row r="296" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A296" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B296" s="5" t="s">
-        <v>380</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="B296" s="5"/>
       <c r="C296" s="5"/>
       <c r="D296" s="5"/>
       <c r="E296" s="5"/>
       <c r="F296" s="5"/>
-      <c r="G296" s="5"/>
+      <c r="G296" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="H296" s="5"/>
       <c r="I296" s="5"/>
       <c r="J296" s="5"/>
-      <c r="K296" s="5"/>
+      <c r="K296" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L296" s="5"/>
-      <c r="M296" s="5"/>
+      <c r="M296" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N296" s="5"/>
-      <c r="O296" s="5"/>
+      <c r="O296" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P296" s="5"/>
       <c r="Q296" s="5"/>
       <c r="R296" s="5"/>
     </row>
     <row r="297" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A297" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="B297" s="5"/>
+        <v>305</v>
+      </c>
+      <c r="B297" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="C297" s="5"/>
       <c r="D297" s="5"/>
       <c r="E297" s="5"/>
@@ -9731,16 +9736,14 @@
       <c r="L297" s="5"/>
       <c r="M297" s="5"/>
       <c r="N297" s="5"/>
-      <c r="O297" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O297" s="5"/>
       <c r="P297" s="5"/>
       <c r="Q297" s="5"/>
       <c r="R297" s="5"/>
     </row>
     <row r="298" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A298" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B298" s="5"/>
       <c r="C298" s="5"/>
@@ -9751,20 +9754,20 @@
       <c r="H298" s="5"/>
       <c r="I298" s="5"/>
       <c r="J298" s="5"/>
-      <c r="K298" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K298" s="5"/>
       <c r="L298" s="5"/>
       <c r="M298" s="5"/>
       <c r="N298" s="5"/>
-      <c r="O298" s="5"/>
+      <c r="O298" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P298" s="5"/>
       <c r="Q298" s="5"/>
       <c r="R298" s="5"/>
     </row>
     <row r="299" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A299" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B299" s="5"/>
       <c r="C299" s="5"/>
@@ -9775,11 +9778,11 @@
       <c r="H299" s="5"/>
       <c r="I299" s="5"/>
       <c r="J299" s="5"/>
-      <c r="K299" s="5"/>
+      <c r="K299" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L299" s="5"/>
-      <c r="M299" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M299" s="5"/>
       <c r="N299" s="5"/>
       <c r="O299" s="5"/>
       <c r="P299" s="5"/>
@@ -9788,7 +9791,7 @@
     </row>
     <row r="300" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A300" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B300" s="5"/>
       <c r="C300" s="5"/>
@@ -9799,9 +9802,7 @@
       <c r="H300" s="5"/>
       <c r="I300" s="5"/>
       <c r="J300" s="5"/>
-      <c r="K300" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K300" s="5"/>
       <c r="L300" s="5"/>
       <c r="M300" s="5" t="s">
         <v>380</v>
@@ -9814,65 +9815,65 @@
     </row>
     <row r="301" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A301" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B301" s="5"/>
       <c r="C301" s="5"/>
       <c r="D301" s="5"/>
       <c r="E301" s="5"/>
-      <c r="F301" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="F301" s="5"/>
       <c r="G301" s="5"/>
-      <c r="H301" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="I301" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="H301" s="5"/>
+      <c r="I301" s="5"/>
       <c r="J301" s="5"/>
-      <c r="K301" s="5"/>
+      <c r="K301" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L301" s="5"/>
-      <c r="M301" s="5"/>
+      <c r="M301" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N301" s="5"/>
       <c r="O301" s="5"/>
-      <c r="P301" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="P301" s="5"/>
       <c r="Q301" s="5"/>
-      <c r="R301" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R301" s="5"/>
     </row>
     <row r="302" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A302" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B302" s="5"/>
       <c r="C302" s="5"/>
       <c r="D302" s="5"/>
       <c r="E302" s="5"/>
-      <c r="F302" s="5"/>
+      <c r="F302" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="G302" s="5"/>
-      <c r="H302" s="5"/>
-      <c r="I302" s="5"/>
+      <c r="H302" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="I302" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="J302" s="5"/>
-      <c r="K302" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="L302" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K302" s="5"/>
+      <c r="L302" s="5"/>
       <c r="M302" s="5"/>
       <c r="N302" s="5"/>
       <c r="O302" s="5"/>
-      <c r="P302" s="5"/>
+      <c r="P302" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q302" s="5"/>
-      <c r="R302" s="5"/>
+      <c r="R302" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="303" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A303" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B303" s="5"/>
       <c r="C303" s="5"/>
@@ -9883,7 +9884,9 @@
       <c r="H303" s="5"/>
       <c r="I303" s="5"/>
       <c r="J303" s="5"/>
-      <c r="K303" s="5"/>
+      <c r="K303" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L303" s="5" t="s">
         <v>380</v>
       </c>
@@ -9896,61 +9899,61 @@
     </row>
     <row r="304" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A304" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B304" s="5"/>
       <c r="C304" s="5"/>
       <c r="D304" s="5"/>
       <c r="E304" s="5"/>
       <c r="F304" s="5"/>
-      <c r="G304" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="G304" s="5"/>
       <c r="H304" s="5"/>
       <c r="I304" s="5"/>
-      <c r="J304" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="J304" s="5"/>
       <c r="K304" s="5"/>
-      <c r="L304" s="5"/>
+      <c r="L304" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="M304" s="5"/>
       <c r="N304" s="5"/>
       <c r="O304" s="5"/>
-      <c r="P304" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="P304" s="5"/>
       <c r="Q304" s="5"/>
-      <c r="R304" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R304" s="5"/>
     </row>
     <row r="305" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A305" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B305" s="5"/>
       <c r="C305" s="5"/>
       <c r="D305" s="5"/>
       <c r="E305" s="5"/>
       <c r="F305" s="5"/>
-      <c r="G305" s="5"/>
+      <c r="G305" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="H305" s="5"/>
       <c r="I305" s="5"/>
-      <c r="J305" s="5"/>
+      <c r="J305" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="K305" s="5"/>
       <c r="L305" s="5"/>
-      <c r="M305" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M305" s="5"/>
       <c r="N305" s="5"/>
       <c r="O305" s="5"/>
-      <c r="P305" s="5"/>
+      <c r="P305" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q305" s="5"/>
-      <c r="R305" s="5"/>
+      <c r="R305" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="306" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A306" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B306" s="5"/>
       <c r="C306" s="5"/>
@@ -9963,18 +9966,18 @@
       <c r="J306" s="5"/>
       <c r="K306" s="5"/>
       <c r="L306" s="5"/>
-      <c r="M306" s="5"/>
+      <c r="M306" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N306" s="5"/>
-      <c r="O306" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O306" s="5"/>
       <c r="P306" s="5"/>
       <c r="Q306" s="5"/>
       <c r="R306" s="5"/>
     </row>
     <row r="307" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A307" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B307" s="5"/>
       <c r="C307" s="5"/>
@@ -9998,7 +10001,7 @@
     </row>
     <row r="308" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A308" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B308" s="5"/>
       <c r="C308" s="5"/>
@@ -10022,15 +10025,13 @@
     </row>
     <row r="309" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A309" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B309" s="5"/>
       <c r="C309" s="5"/>
       <c r="D309" s="5"/>
       <c r="E309" s="5"/>
-      <c r="F309" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="F309" s="5"/>
       <c r="G309" s="5"/>
       <c r="H309" s="5"/>
       <c r="I309" s="5"/>
@@ -10039,36 +10040,32 @@
       <c r="L309" s="5"/>
       <c r="M309" s="5"/>
       <c r="N309" s="5"/>
-      <c r="O309" s="5"/>
+      <c r="O309" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P309" s="5"/>
       <c r="Q309" s="5"/>
       <c r="R309" s="5"/>
     </row>
     <row r="310" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A310" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="B310" s="5" t="s">
-        <v>380</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="B310" s="5"/>
       <c r="C310" s="5"/>
       <c r="D310" s="5"/>
       <c r="E310" s="5"/>
-      <c r="F310" s="5"/>
+      <c r="F310" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="G310" s="5"/>
       <c r="H310" s="5"/>
       <c r="I310" s="5"/>
       <c r="J310" s="5"/>
-      <c r="K310" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K310" s="5"/>
       <c r="L310" s="5"/>
-      <c r="M310" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="N310" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M310" s="5"/>
+      <c r="N310" s="5"/>
       <c r="O310" s="5"/>
       <c r="P310" s="5"/>
       <c r="Q310" s="5"/>
@@ -10076,9 +10073,11 @@
     </row>
     <row r="311" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A311" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="B311" s="5"/>
+        <v>319</v>
+      </c>
+      <c r="B311" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="C311" s="5"/>
       <c r="D311" s="5"/>
       <c r="E311" s="5"/>
@@ -10087,12 +10086,16 @@
       <c r="H311" s="5"/>
       <c r="I311" s="5"/>
       <c r="J311" s="5"/>
-      <c r="K311" s="5"/>
-      <c r="L311" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="M311" s="5"/>
-      <c r="N311" s="5"/>
+      <c r="K311" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="L311" s="5"/>
+      <c r="M311" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="N311" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="O311" s="5"/>
       <c r="P311" s="5"/>
       <c r="Q311" s="5"/>
@@ -10100,7 +10103,7 @@
     </row>
     <row r="312" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A312" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B312" s="5"/>
       <c r="C312" s="5"/>
@@ -10111,22 +10114,20 @@
       <c r="H312" s="5"/>
       <c r="I312" s="5"/>
       <c r="J312" s="5"/>
-      <c r="K312" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="L312" s="5"/>
+      <c r="K312" s="5"/>
+      <c r="L312" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="M312" s="5"/>
       <c r="N312" s="5"/>
-      <c r="O312" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O312" s="5"/>
       <c r="P312" s="5"/>
       <c r="Q312" s="5"/>
       <c r="R312" s="5"/>
     </row>
     <row r="313" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A313" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B313" s="5"/>
       <c r="C313" s="5"/>
@@ -10143,14 +10144,16 @@
       <c r="L313" s="5"/>
       <c r="M313" s="5"/>
       <c r="N313" s="5"/>
-      <c r="O313" s="5"/>
+      <c r="O313" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P313" s="5"/>
       <c r="Q313" s="5"/>
       <c r="R313" s="5"/>
     </row>
     <row r="314" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A314" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B314" s="5"/>
       <c r="C314" s="5"/>
@@ -10161,20 +10164,20 @@
       <c r="H314" s="5"/>
       <c r="I314" s="5"/>
       <c r="J314" s="5"/>
-      <c r="K314" s="5"/>
+      <c r="K314" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L314" s="5"/>
       <c r="M314" s="5"/>
       <c r="N314" s="5"/>
       <c r="O314" s="5"/>
       <c r="P314" s="5"/>
       <c r="Q314" s="5"/>
-      <c r="R314" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R314" s="5"/>
     </row>
     <row r="315" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A315" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B315" s="5"/>
       <c r="C315" s="5"/>
@@ -10188,17 +10191,17 @@
       <c r="K315" s="5"/>
       <c r="L315" s="5"/>
       <c r="M315" s="5"/>
-      <c r="N315" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="N315" s="5"/>
       <c r="O315" s="5"/>
       <c r="P315" s="5"/>
       <c r="Q315" s="5"/>
-      <c r="R315" s="5"/>
+      <c r="R315" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="316" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A316" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B316" s="5"/>
       <c r="C316" s="5"/>
@@ -10211,10 +10214,10 @@
       <c r="J316" s="5"/>
       <c r="K316" s="5"/>
       <c r="L316" s="5"/>
-      <c r="M316" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="N316" s="5"/>
+      <c r="M316" s="5"/>
+      <c r="N316" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="O316" s="5"/>
       <c r="P316" s="5"/>
       <c r="Q316" s="5"/>
@@ -10222,22 +10225,22 @@
     </row>
     <row r="317" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A317" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B317" s="5"/>
       <c r="C317" s="5"/>
       <c r="D317" s="5"/>
       <c r="E317" s="5"/>
       <c r="F317" s="5"/>
-      <c r="G317" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="G317" s="5"/>
       <c r="H317" s="5"/>
       <c r="I317" s="5"/>
       <c r="J317" s="5"/>
       <c r="K317" s="5"/>
       <c r="L317" s="5"/>
-      <c r="M317" s="5"/>
+      <c r="M317" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N317" s="5"/>
       <c r="O317" s="5"/>
       <c r="P317" s="5"/>
@@ -10246,16 +10249,16 @@
     </row>
     <row r="318" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A318" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B318" s="5"/>
       <c r="C318" s="5"/>
-      <c r="D318" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="D318" s="5"/>
       <c r="E318" s="5"/>
       <c r="F318" s="5"/>
-      <c r="G318" s="5"/>
+      <c r="G318" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="H318" s="5"/>
       <c r="I318" s="5"/>
       <c r="J318" s="5"/>
@@ -10270,11 +10273,13 @@
     </row>
     <row r="319" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A319" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B319" s="5"/>
       <c r="C319" s="5"/>
-      <c r="D319" s="5"/>
+      <c r="D319" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="E319" s="5"/>
       <c r="F319" s="5"/>
       <c r="G319" s="5"/>
@@ -10283,20 +10288,16 @@
       <c r="J319" s="5"/>
       <c r="K319" s="5"/>
       <c r="L319" s="5"/>
-      <c r="M319" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M319" s="5"/>
       <c r="N319" s="5"/>
-      <c r="O319" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O319" s="5"/>
       <c r="P319" s="5"/>
       <c r="Q319" s="5"/>
       <c r="R319" s="5"/>
     </row>
     <row r="320" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A320" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B320" s="5"/>
       <c r="C320" s="5"/>
@@ -10313,14 +10314,16 @@
         <v>380</v>
       </c>
       <c r="N320" s="5"/>
-      <c r="O320" s="5"/>
+      <c r="O320" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P320" s="5"/>
       <c r="Q320" s="5"/>
       <c r="R320" s="5"/>
     </row>
     <row r="321" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A321" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B321" s="5"/>
       <c r="C321" s="5"/>
@@ -10329,59 +10332,61 @@
       <c r="F321" s="5"/>
       <c r="G321" s="5"/>
       <c r="H321" s="5"/>
-      <c r="I321" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J321" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="I321" s="5"/>
+      <c r="J321" s="5"/>
       <c r="K321" s="5"/>
-      <c r="L321" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="L321" s="5"/>
       <c r="M321" s="5" t="s">
         <v>380</v>
       </c>
       <c r="N321" s="5"/>
-      <c r="O321" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O321" s="5"/>
       <c r="P321" s="5"/>
       <c r="Q321" s="5"/>
       <c r="R321" s="5"/>
     </row>
     <row r="322" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A322" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B322" s="5"/>
       <c r="C322" s="5"/>
       <c r="D322" s="5"/>
-      <c r="E322" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="E322" s="5"/>
       <c r="F322" s="5"/>
       <c r="G322" s="5"/>
       <c r="H322" s="5"/>
-      <c r="I322" s="5"/>
-      <c r="J322" s="5"/>
+      <c r="I322" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J322" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="K322" s="5"/>
-      <c r="L322" s="5"/>
-      <c r="M322" s="5"/>
+      <c r="L322" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="M322" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N322" s="5"/>
-      <c r="O322" s="5"/>
+      <c r="O322" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P322" s="5"/>
       <c r="Q322" s="5"/>
       <c r="R322" s="5"/>
     </row>
     <row r="323" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A323" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B323" s="5"/>
       <c r="C323" s="5"/>
       <c r="D323" s="5"/>
-      <c r="E323" s="5"/>
+      <c r="E323" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="F323" s="5"/>
       <c r="G323" s="5"/>
       <c r="H323" s="5"/>
@@ -10394,13 +10399,11 @@
       <c r="O323" s="5"/>
       <c r="P323" s="5"/>
       <c r="Q323" s="5"/>
-      <c r="R323" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R323" s="5"/>
     </row>
     <row r="324" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A324" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B324" s="5"/>
       <c r="C324" s="5"/>
@@ -10411,9 +10414,7 @@
       <c r="H324" s="5"/>
       <c r="I324" s="5"/>
       <c r="J324" s="5"/>
-      <c r="K324" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K324" s="5"/>
       <c r="L324" s="5"/>
       <c r="M324" s="5"/>
       <c r="N324" s="5"/>
@@ -10426,7 +10427,7 @@
     </row>
     <row r="325" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A325" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B325" s="5"/>
       <c r="C325" s="5"/>
@@ -10436,21 +10437,23 @@
       <c r="G325" s="5"/>
       <c r="H325" s="5"/>
       <c r="I325" s="5"/>
-      <c r="J325" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="K325" s="5"/>
+      <c r="J325" s="5"/>
+      <c r="K325" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L325" s="5"/>
       <c r="M325" s="5"/>
       <c r="N325" s="5"/>
       <c r="O325" s="5"/>
       <c r="P325" s="5"/>
       <c r="Q325" s="5"/>
-      <c r="R325" s="5"/>
+      <c r="R325" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="326" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A326" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B326" s="5"/>
       <c r="C326" s="5"/>
@@ -10460,10 +10463,10 @@
       <c r="G326" s="5"/>
       <c r="H326" s="5"/>
       <c r="I326" s="5"/>
-      <c r="J326" s="5"/>
-      <c r="K326" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="J326" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="K326" s="5"/>
       <c r="L326" s="5"/>
       <c r="M326" s="5"/>
       <c r="N326" s="5"/>
@@ -10474,20 +10477,20 @@
     </row>
     <row r="327" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A327" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B327" s="5"/>
       <c r="C327" s="5"/>
       <c r="D327" s="5"/>
-      <c r="E327" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="E327" s="5"/>
       <c r="F327" s="5"/>
       <c r="G327" s="5"/>
       <c r="H327" s="5"/>
       <c r="I327" s="5"/>
       <c r="J327" s="5"/>
-      <c r="K327" s="5"/>
+      <c r="K327" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L327" s="5"/>
       <c r="M327" s="5"/>
       <c r="N327" s="5"/>
@@ -10498,14 +10501,14 @@
     </row>
     <row r="328" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A328" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B328" s="5"/>
       <c r="C328" s="5"/>
-      <c r="D328" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="E328" s="5"/>
+      <c r="D328" s="5"/>
+      <c r="E328" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="F328" s="5"/>
       <c r="G328" s="5"/>
       <c r="H328" s="5"/>
@@ -10514,23 +10517,21 @@
       <c r="K328" s="5"/>
       <c r="L328" s="5"/>
       <c r="M328" s="5"/>
-      <c r="N328" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="N328" s="5"/>
       <c r="O328" s="5"/>
       <c r="P328" s="5"/>
-      <c r="Q328" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="Q328" s="5"/>
       <c r="R328" s="5"/>
     </row>
     <row r="329" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A329" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B329" s="5"/>
       <c r="C329" s="5"/>
-      <c r="D329" s="5"/>
+      <c r="D329" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="E329" s="5"/>
       <c r="F329" s="5"/>
       <c r="G329" s="5"/>
@@ -10540,73 +10541,75 @@
       <c r="K329" s="5"/>
       <c r="L329" s="5"/>
       <c r="M329" s="5"/>
-      <c r="N329" s="5"/>
+      <c r="N329" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="O329" s="5"/>
       <c r="P329" s="5"/>
-      <c r="Q329" s="5"/>
-      <c r="R329" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="Q329" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="R329" s="5"/>
     </row>
     <row r="330" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B330" s="5"/>
-      <c r="C330" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="C330" s="5"/>
       <c r="D330" s="5"/>
       <c r="E330" s="5"/>
       <c r="F330" s="5"/>
       <c r="G330" s="5"/>
       <c r="H330" s="5"/>
       <c r="I330" s="5"/>
-      <c r="J330" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="J330" s="5"/>
       <c r="K330" s="5"/>
       <c r="L330" s="5"/>
       <c r="M330" s="5"/>
       <c r="N330" s="5"/>
-      <c r="O330" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="P330" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q330" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="R330" s="5"/>
+      <c r="O330" s="5"/>
+      <c r="P330" s="5"/>
+      <c r="Q330" s="5"/>
+      <c r="R330" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="331" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A331" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B331" s="5"/>
-      <c r="C331" s="5"/>
+      <c r="C331" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="D331" s="5"/>
       <c r="E331" s="5"/>
       <c r="F331" s="5"/>
       <c r="G331" s="5"/>
       <c r="H331" s="5"/>
       <c r="I331" s="5"/>
-      <c r="J331" s="5"/>
+      <c r="J331" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="K331" s="5"/>
       <c r="L331" s="5"/>
-      <c r="M331" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M331" s="5"/>
       <c r="N331" s="5"/>
-      <c r="O331" s="5"/>
-      <c r="P331" s="5"/>
-      <c r="Q331" s="5"/>
+      <c r="O331" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="P331" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q331" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="R331" s="5"/>
     </row>
     <row r="332" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B332" s="5"/>
       <c r="C332" s="5"/>
@@ -10619,28 +10622,24 @@
       <c r="J332" s="5"/>
       <c r="K332" s="5"/>
       <c r="L332" s="5"/>
-      <c r="M332" s="5"/>
+      <c r="M332" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N332" s="5"/>
       <c r="O332" s="5"/>
       <c r="P332" s="5"/>
       <c r="Q332" s="5"/>
-      <c r="R332" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R332" s="5"/>
     </row>
     <row r="333" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A333" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B333" s="5"/>
-      <c r="C333" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="C333" s="5"/>
       <c r="D333" s="5"/>
       <c r="E333" s="5"/>
-      <c r="F333" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="F333" s="5"/>
       <c r="G333" s="5"/>
       <c r="H333" s="5"/>
       <c r="I333" s="5"/>
@@ -10652,43 +10651,39 @@
       <c r="O333" s="5"/>
       <c r="P333" s="5"/>
       <c r="Q333" s="5"/>
-      <c r="R333" s="5"/>
+      <c r="R333" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="334" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A334" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B334" s="5"/>
-      <c r="C334" s="5"/>
+      <c r="C334" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="D334" s="5"/>
       <c r="E334" s="5"/>
-      <c r="F334" s="5"/>
+      <c r="F334" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="G334" s="5"/>
       <c r="H334" s="5"/>
-      <c r="I334" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="I334" s="5"/>
       <c r="J334" s="5"/>
       <c r="K334" s="5"/>
       <c r="L334" s="5"/>
-      <c r="M334" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M334" s="5"/>
       <c r="N334" s="5"/>
-      <c r="O334" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="P334" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O334" s="5"/>
+      <c r="P334" s="5"/>
       <c r="Q334" s="5"/>
-      <c r="R334" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R334" s="5"/>
     </row>
     <row r="335" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A335" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B335" s="5"/>
       <c r="C335" s="5"/>
@@ -10697,14 +10692,22 @@
       <c r="F335" s="5"/>
       <c r="G335" s="5"/>
       <c r="H335" s="5"/>
-      <c r="I335" s="5"/>
+      <c r="I335" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="J335" s="5"/>
       <c r="K335" s="5"/>
       <c r="L335" s="5"/>
-      <c r="M335" s="5"/>
+      <c r="M335" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N335" s="5"/>
-      <c r="O335" s="5"/>
-      <c r="P335" s="5"/>
+      <c r="O335" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="P335" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q335" s="5"/>
       <c r="R335" s="5" t="s">
         <v>380</v>
@@ -10712,73 +10715,73 @@
     </row>
     <row r="336" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A336" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="B336" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="C336" s="5" t="s">
-        <v>380</v>
-      </c>
+        <v>344</v>
+      </c>
+      <c r="B336" s="5"/>
+      <c r="C336" s="5"/>
       <c r="D336" s="5"/>
       <c r="E336" s="5"/>
-      <c r="F336" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="G336" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="F336" s="5"/>
+      <c r="G336" s="5"/>
       <c r="H336" s="5"/>
-      <c r="I336" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J336" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="K336" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="I336" s="5"/>
+      <c r="J336" s="5"/>
+      <c r="K336" s="5"/>
       <c r="L336" s="5"/>
-      <c r="M336" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M336" s="5"/>
       <c r="N336" s="5"/>
-      <c r="O336" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="P336" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O336" s="5"/>
+      <c r="P336" s="5"/>
       <c r="Q336" s="5"/>
-      <c r="R336" s="5"/>
+      <c r="R336" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="337" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A337" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="B337" s="5"/>
-      <c r="C337" s="5"/>
+        <v>345</v>
+      </c>
+      <c r="B337" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="C337" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="D337" s="5"/>
       <c r="E337" s="5"/>
-      <c r="F337" s="5"/>
-      <c r="G337" s="5"/>
+      <c r="F337" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="G337" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="H337" s="5"/>
-      <c r="I337" s="5"/>
-      <c r="J337" s="5"/>
-      <c r="K337" s="5"/>
+      <c r="I337" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J337" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="K337" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L337" s="5"/>
       <c r="M337" s="5" t="s">
         <v>380</v>
       </c>
       <c r="N337" s="5"/>
-      <c r="O337" s="5"/>
-      <c r="P337" s="5"/>
+      <c r="O337" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="P337" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q337" s="5"/>
       <c r="R337" s="5"/>
     </row>
     <row r="338" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A338" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B338" s="5"/>
       <c r="C338" s="5"/>
@@ -10790,10 +10793,10 @@
       <c r="I338" s="5"/>
       <c r="J338" s="5"/>
       <c r="K338" s="5"/>
-      <c r="L338" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="M338" s="5"/>
+      <c r="L338" s="5"/>
+      <c r="M338" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N338" s="5"/>
       <c r="O338" s="5"/>
       <c r="P338" s="5"/>
@@ -10802,7 +10805,7 @@
     </row>
     <row r="339" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A339" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B339" s="5"/>
       <c r="C339" s="5"/>
@@ -10826,94 +10829,94 @@
     </row>
     <row r="340" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A340" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B340" s="5"/>
-      <c r="C340" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="C340" s="5"/>
       <c r="D340" s="5"/>
-      <c r="E340" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="E340" s="5"/>
       <c r="F340" s="5"/>
       <c r="G340" s="5"/>
       <c r="H340" s="5"/>
-      <c r="I340" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J340" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="I340" s="5"/>
+      <c r="J340" s="5"/>
       <c r="K340" s="5"/>
       <c r="L340" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="M340" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M340" s="5"/>
       <c r="N340" s="5"/>
-      <c r="O340" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="P340" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O340" s="5"/>
+      <c r="P340" s="5"/>
       <c r="Q340" s="5"/>
-      <c r="R340" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R340" s="5"/>
     </row>
     <row r="341" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A341" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="B341" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="C341" s="5"/>
+        <v>349</v>
+      </c>
+      <c r="B341" s="5"/>
+      <c r="C341" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="D341" s="5"/>
-      <c r="E341" s="5"/>
-      <c r="F341" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="E341" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="F341" s="5"/>
       <c r="G341" s="5"/>
-      <c r="H341" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="I341" s="5"/>
-      <c r="J341" s="5"/>
-      <c r="K341" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="L341" s="5"/>
+      <c r="H341" s="5"/>
+      <c r="I341" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J341" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="K341" s="5"/>
+      <c r="L341" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="M341" s="5" t="s">
         <v>380</v>
       </c>
       <c r="N341" s="5"/>
-      <c r="O341" s="5"/>
-      <c r="P341" s="5"/>
+      <c r="O341" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="P341" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q341" s="5"/>
-      <c r="R341" s="5"/>
+      <c r="R341" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="342" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A342" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="B342" s="5"/>
+        <v>350</v>
+      </c>
+      <c r="B342" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="C342" s="5"/>
       <c r="D342" s="5"/>
       <c r="E342" s="5"/>
-      <c r="F342" s="5"/>
-      <c r="G342" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="H342" s="5"/>
+      <c r="F342" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="G342" s="5"/>
+      <c r="H342" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="I342" s="5"/>
       <c r="J342" s="5"/>
-      <c r="K342" s="5"/>
+      <c r="K342" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L342" s="5"/>
-      <c r="M342" s="5"/>
+      <c r="M342" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N342" s="5"/>
       <c r="O342" s="5"/>
       <c r="P342" s="5"/>
@@ -10922,15 +10925,11 @@
     </row>
     <row r="343" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A343" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="B343" s="5" t="s">
-        <v>380</v>
-      </c>
+        <v>351</v>
+      </c>
+      <c r="B343" s="5"/>
       <c r="C343" s="5"/>
-      <c r="D343" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="D343" s="5"/>
       <c r="E343" s="5"/>
       <c r="F343" s="5"/>
       <c r="G343" s="5" t="s">
@@ -10939,35 +10938,31 @@
       <c r="H343" s="5"/>
       <c r="I343" s="5"/>
       <c r="J343" s="5"/>
-      <c r="K343" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K343" s="5"/>
       <c r="L343" s="5"/>
-      <c r="M343" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M343" s="5"/>
       <c r="N343" s="5"/>
-      <c r="O343" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O343" s="5"/>
       <c r="P343" s="5"/>
-      <c r="Q343" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="R343" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="Q343" s="5"/>
+      <c r="R343" s="5"/>
     </row>
     <row r="344" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A344" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="B344" s="5"/>
+        <v>352</v>
+      </c>
+      <c r="B344" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="C344" s="5"/>
-      <c r="D344" s="5"/>
+      <c r="D344" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="E344" s="5"/>
       <c r="F344" s="5"/>
-      <c r="G344" s="5"/>
+      <c r="G344" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="H344" s="5"/>
       <c r="I344" s="5"/>
       <c r="J344" s="5"/>
@@ -10975,16 +10970,24 @@
         <v>380</v>
       </c>
       <c r="L344" s="5"/>
-      <c r="M344" s="5"/>
+      <c r="M344" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N344" s="5"/>
-      <c r="O344" s="5"/>
+      <c r="O344" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P344" s="5"/>
-      <c r="Q344" s="5"/>
-      <c r="R344" s="5"/>
+      <c r="Q344" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="R344" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="345" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A345" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B345" s="5"/>
       <c r="C345" s="5"/>
@@ -10995,20 +10998,20 @@
       <c r="H345" s="5"/>
       <c r="I345" s="5"/>
       <c r="J345" s="5"/>
-      <c r="K345" s="5"/>
+      <c r="K345" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L345" s="5"/>
       <c r="M345" s="5"/>
       <c r="N345" s="5"/>
       <c r="O345" s="5"/>
       <c r="P345" s="5"/>
       <c r="Q345" s="5"/>
-      <c r="R345" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R345" s="5"/>
     </row>
     <row r="346" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A346" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B346" s="5"/>
       <c r="C346" s="5"/>
@@ -11016,9 +11019,7 @@
       <c r="E346" s="5"/>
       <c r="F346" s="5"/>
       <c r="G346" s="5"/>
-      <c r="H346" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="H346" s="5"/>
       <c r="I346" s="5"/>
       <c r="J346" s="5"/>
       <c r="K346" s="5"/>
@@ -11028,11 +11029,13 @@
       <c r="O346" s="5"/>
       <c r="P346" s="5"/>
       <c r="Q346" s="5"/>
-      <c r="R346" s="5"/>
+      <c r="R346" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="347" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A347" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B347" s="5"/>
       <c r="C347" s="5"/>
@@ -11040,15 +11043,15 @@
       <c r="E347" s="5"/>
       <c r="F347" s="5"/>
       <c r="G347" s="5"/>
-      <c r="H347" s="5"/>
+      <c r="H347" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="I347" s="5"/>
       <c r="J347" s="5"/>
       <c r="K347" s="5"/>
       <c r="L347" s="5"/>
       <c r="M347" s="5"/>
-      <c r="N347" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="N347" s="5"/>
       <c r="O347" s="5"/>
       <c r="P347" s="5"/>
       <c r="Q347" s="5"/>
@@ -11056,7 +11059,7 @@
     </row>
     <row r="348" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A348" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B348" s="5"/>
       <c r="C348" s="5"/>
@@ -11064,15 +11067,15 @@
       <c r="E348" s="5"/>
       <c r="F348" s="5"/>
       <c r="G348" s="5"/>
-      <c r="H348" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="H348" s="5"/>
       <c r="I348" s="5"/>
       <c r="J348" s="5"/>
       <c r="K348" s="5"/>
       <c r="L348" s="5"/>
       <c r="M348" s="5"/>
-      <c r="N348" s="5"/>
+      <c r="N348" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="O348" s="5"/>
       <c r="P348" s="5"/>
       <c r="Q348" s="5"/>
@@ -11080,7 +11083,7 @@
     </row>
     <row r="349" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A349" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B349" s="5"/>
       <c r="C349" s="5"/>
@@ -11088,15 +11091,15 @@
       <c r="E349" s="5"/>
       <c r="F349" s="5"/>
       <c r="G349" s="5"/>
-      <c r="H349" s="5"/>
+      <c r="H349" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="I349" s="5"/>
       <c r="J349" s="5"/>
       <c r="K349" s="5"/>
       <c r="L349" s="5"/>
       <c r="M349" s="5"/>
-      <c r="N349" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="N349" s="5"/>
       <c r="O349" s="5"/>
       <c r="P349" s="5"/>
       <c r="Q349" s="5"/>
@@ -11104,7 +11107,7 @@
     </row>
     <row r="350" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A350" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B350" s="5"/>
       <c r="C350" s="5"/>
@@ -11117,22 +11120,18 @@
       <c r="J350" s="5"/>
       <c r="K350" s="5"/>
       <c r="L350" s="5"/>
-      <c r="M350" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="N350" s="5"/>
+      <c r="M350" s="5"/>
+      <c r="N350" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="O350" s="5"/>
       <c r="P350" s="5"/>
-      <c r="Q350" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="R350" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="Q350" s="5"/>
+      <c r="R350" s="5"/>
     </row>
     <row r="351" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A351" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B351" s="5"/>
       <c r="C351" s="5"/>
@@ -11145,24 +11144,26 @@
       <c r="J351" s="5"/>
       <c r="K351" s="5"/>
       <c r="L351" s="5"/>
-      <c r="M351" s="5"/>
+      <c r="M351" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N351" s="5"/>
       <c r="O351" s="5"/>
       <c r="P351" s="5"/>
-      <c r="Q351" s="5"/>
+      <c r="Q351" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="R351" s="5" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="352" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A352" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B352" s="5"/>
       <c r="C352" s="5"/>
-      <c r="D352" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="D352" s="5"/>
       <c r="E352" s="5"/>
       <c r="F352" s="5"/>
       <c r="G352" s="5"/>
@@ -11171,9 +11172,7 @@
       <c r="J352" s="5"/>
       <c r="K352" s="5"/>
       <c r="L352" s="5"/>
-      <c r="M352" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M352" s="5"/>
       <c r="N352" s="5"/>
       <c r="O352" s="5"/>
       <c r="P352" s="5"/>
@@ -11184,11 +11183,13 @@
     </row>
     <row r="353" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A353" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B353" s="5"/>
       <c r="C353" s="5"/>
-      <c r="D353" s="5"/>
+      <c r="D353" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="E353" s="5"/>
       <c r="F353" s="5"/>
       <c r="G353" s="5"/>
@@ -11197,57 +11198,59 @@
       <c r="J353" s="5"/>
       <c r="K353" s="5"/>
       <c r="L353" s="5"/>
-      <c r="M353" s="5"/>
+      <c r="M353" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N353" s="5"/>
-      <c r="O353" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O353" s="5"/>
       <c r="P353" s="5"/>
       <c r="Q353" s="5"/>
-      <c r="R353" s="5"/>
+      <c r="R353" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="354" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A354" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B354" s="5"/>
       <c r="C354" s="5"/>
-      <c r="D354" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="D354" s="5"/>
       <c r="E354" s="5"/>
       <c r="F354" s="5"/>
       <c r="G354" s="5"/>
       <c r="H354" s="5"/>
       <c r="I354" s="5"/>
       <c r="J354" s="5"/>
-      <c r="K354" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K354" s="5"/>
       <c r="L354" s="5"/>
       <c r="M354" s="5"/>
       <c r="N354" s="5"/>
-      <c r="O354" s="5"/>
+      <c r="O354" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P354" s="5"/>
       <c r="Q354" s="5"/>
       <c r="R354" s="5"/>
     </row>
     <row r="355" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A355" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B355" s="5"/>
       <c r="C355" s="5"/>
-      <c r="D355" s="5"/>
+      <c r="D355" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="E355" s="5"/>
       <c r="F355" s="5"/>
       <c r="G355" s="5"/>
       <c r="H355" s="5"/>
-      <c r="I355" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="I355" s="5"/>
       <c r="J355" s="5"/>
-      <c r="K355" s="5"/>
+      <c r="K355" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L355" s="5"/>
       <c r="M355" s="5"/>
       <c r="N355" s="5"/>
@@ -11258,7 +11261,7 @@
     </row>
     <row r="356" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A356" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B356" s="5"/>
       <c r="C356" s="5"/>
@@ -11267,10 +11270,10 @@
       <c r="F356" s="5"/>
       <c r="G356" s="5"/>
       <c r="H356" s="5"/>
-      <c r="I356" s="5"/>
-      <c r="J356" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="I356" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="J356" s="5"/>
       <c r="K356" s="5"/>
       <c r="L356" s="5"/>
       <c r="M356" s="5"/>
@@ -11282,40 +11285,40 @@
     </row>
     <row r="357" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A357" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B357" s="5"/>
       <c r="C357" s="5"/>
       <c r="D357" s="5"/>
       <c r="E357" s="5"/>
       <c r="F357" s="5"/>
-      <c r="G357" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="G357" s="5"/>
       <c r="H357" s="5"/>
       <c r="I357" s="5"/>
-      <c r="J357" s="5"/>
+      <c r="J357" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="K357" s="5"/>
       <c r="L357" s="5"/>
       <c r="M357" s="5"/>
       <c r="N357" s="5"/>
       <c r="O357" s="5"/>
-      <c r="P357" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="P357" s="5"/>
       <c r="Q357" s="5"/>
       <c r="R357" s="5"/>
     </row>
     <row r="358" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A358" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B358" s="5"/>
       <c r="C358" s="5"/>
       <c r="D358" s="5"/>
       <c r="E358" s="5"/>
       <c r="F358" s="5"/>
-      <c r="G358" s="5"/>
+      <c r="G358" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="H358" s="5"/>
       <c r="I358" s="5"/>
       <c r="J358" s="5"/>
@@ -11323,16 +11326,16 @@
       <c r="L358" s="5"/>
       <c r="M358" s="5"/>
       <c r="N358" s="5"/>
-      <c r="O358" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="P358" s="5"/>
+      <c r="O358" s="5"/>
+      <c r="P358" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q358" s="5"/>
       <c r="R358" s="5"/>
     </row>
     <row r="359" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A359" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B359" s="5"/>
       <c r="C359" s="5"/>
@@ -11343,20 +11346,20 @@
       <c r="H359" s="5"/>
       <c r="I359" s="5"/>
       <c r="J359" s="5"/>
-      <c r="K359" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K359" s="5"/>
       <c r="L359" s="5"/>
       <c r="M359" s="5"/>
       <c r="N359" s="5"/>
-      <c r="O359" s="5"/>
+      <c r="O359" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P359" s="5"/>
       <c r="Q359" s="5"/>
       <c r="R359" s="5"/>
     </row>
     <row r="360" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A360" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B360" s="5"/>
       <c r="C360" s="5"/>
@@ -11367,24 +11370,20 @@
       <c r="H360" s="5"/>
       <c r="I360" s="5"/>
       <c r="J360" s="5"/>
-      <c r="K360" s="5"/>
+      <c r="K360" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L360" s="5"/>
-      <c r="M360" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="M360" s="5"/>
       <c r="N360" s="5"/>
-      <c r="O360" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O360" s="5"/>
       <c r="P360" s="5"/>
-      <c r="Q360" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="Q360" s="5"/>
       <c r="R360" s="5"/>
     </row>
     <row r="361" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A361" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B361" s="5"/>
       <c r="C361" s="5"/>
@@ -11395,22 +11394,24 @@
       <c r="H361" s="5"/>
       <c r="I361" s="5"/>
       <c r="J361" s="5"/>
-      <c r="K361" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="K361" s="5"/>
       <c r="L361" s="5"/>
-      <c r="M361" s="5"/>
+      <c r="M361" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="N361" s="5"/>
       <c r="O361" s="5" t="s">
         <v>380</v>
       </c>
       <c r="P361" s="5"/>
-      <c r="Q361" s="5"/>
+      <c r="Q361" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="R361" s="5"/>
     </row>
     <row r="362" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A362" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B362" s="5"/>
       <c r="C362" s="5"/>
@@ -11421,20 +11422,22 @@
       <c r="H362" s="5"/>
       <c r="I362" s="5"/>
       <c r="J362" s="5"/>
-      <c r="K362" s="5"/>
+      <c r="K362" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L362" s="5"/>
       <c r="M362" s="5"/>
       <c r="N362" s="5"/>
-      <c r="O362" s="5"/>
-      <c r="P362" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O362" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="P362" s="5"/>
       <c r="Q362" s="5"/>
       <c r="R362" s="5"/>
     </row>
     <row r="363" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A363" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B363" s="5"/>
       <c r="C363" s="5"/>
@@ -11449,16 +11452,16 @@
       <c r="L363" s="5"/>
       <c r="M363" s="5"/>
       <c r="N363" s="5"/>
-      <c r="O363" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="P363" s="5"/>
+      <c r="O363" s="5"/>
+      <c r="P363" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="Q363" s="5"/>
       <c r="R363" s="5"/>
     </row>
     <row r="364" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A364" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B364" s="5"/>
       <c r="C364" s="5"/>
@@ -11482,7 +11485,7 @@
     </row>
     <row r="365" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A365" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B365" s="5"/>
       <c r="C365" s="5"/>
@@ -11494,19 +11497,19 @@
       <c r="I365" s="5"/>
       <c r="J365" s="5"/>
       <c r="K365" s="5"/>
-      <c r="L365" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="L365" s="5"/>
       <c r="M365" s="5"/>
       <c r="N365" s="5"/>
-      <c r="O365" s="5"/>
+      <c r="O365" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="P365" s="5"/>
       <c r="Q365" s="5"/>
       <c r="R365" s="5"/>
     </row>
     <row r="366" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A366" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B366" s="5"/>
       <c r="C366" s="5"/>
@@ -11516,23 +11519,21 @@
       <c r="G366" s="5"/>
       <c r="H366" s="5"/>
       <c r="I366" s="5"/>
-      <c r="J366" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="J366" s="5"/>
       <c r="K366" s="5"/>
-      <c r="L366" s="5"/>
+      <c r="L366" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="M366" s="5"/>
       <c r="N366" s="5"/>
       <c r="O366" s="5"/>
       <c r="P366" s="5"/>
       <c r="Q366" s="5"/>
-      <c r="R366" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R366" s="5"/>
     </row>
     <row r="367" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A367" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B367" s="5"/>
       <c r="C367" s="5"/>
@@ -11542,21 +11543,23 @@
       <c r="G367" s="5"/>
       <c r="H367" s="5"/>
       <c r="I367" s="5"/>
-      <c r="J367" s="5"/>
-      <c r="K367" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="J367" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="K367" s="5"/>
       <c r="L367" s="5"/>
       <c r="M367" s="5"/>
       <c r="N367" s="5"/>
       <c r="O367" s="5"/>
       <c r="P367" s="5"/>
       <c r="Q367" s="5"/>
-      <c r="R367" s="5"/>
+      <c r="R367" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="368" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A368" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B368" s="5"/>
       <c r="C368" s="5"/>
@@ -11566,23 +11569,21 @@
       <c r="G368" s="5"/>
       <c r="H368" s="5"/>
       <c r="I368" s="5"/>
-      <c r="J368" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="K368" s="5"/>
+      <c r="J368" s="5"/>
+      <c r="K368" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="L368" s="5"/>
       <c r="M368" s="5"/>
       <c r="N368" s="5"/>
       <c r="O368" s="5"/>
       <c r="P368" s="5"/>
       <c r="Q368" s="5"/>
-      <c r="R368" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="R368" s="5"/>
     </row>
     <row r="369" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A369" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B369" s="5"/>
       <c r="C369" s="5"/>
@@ -11602,11 +11603,13 @@
       <c r="O369" s="5"/>
       <c r="P369" s="5"/>
       <c r="Q369" s="5"/>
-      <c r="R369" s="5"/>
+      <c r="R369" s="5" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="370" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A370" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B370" s="5"/>
       <c r="C370" s="5"/>
@@ -11616,17 +11619,41 @@
       <c r="G370" s="5"/>
       <c r="H370" s="5"/>
       <c r="I370" s="5"/>
-      <c r="J370" s="5"/>
+      <c r="J370" s="5" t="s">
+        <v>380</v>
+      </c>
       <c r="K370" s="5"/>
       <c r="L370" s="5"/>
       <c r="M370" s="5"/>
       <c r="N370" s="5"/>
-      <c r="O370" s="5" t="s">
-        <v>380</v>
-      </c>
+      <c r="O370" s="5"/>
       <c r="P370" s="5"/>
       <c r="Q370" s="5"/>
       <c r="R370" s="5"/>
+    </row>
+    <row r="371" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A371" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B371" s="5"/>
+      <c r="C371" s="5"/>
+      <c r="D371" s="5"/>
+      <c r="E371" s="5"/>
+      <c r="F371" s="5"/>
+      <c r="G371" s="5"/>
+      <c r="H371" s="5"/>
+      <c r="I371" s="5"/>
+      <c r="J371" s="5"/>
+      <c r="K371" s="5"/>
+      <c r="L371" s="5"/>
+      <c r="M371" s="5"/>
+      <c r="N371" s="5"/>
+      <c r="O371" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="P371" s="5"/>
+      <c r="Q371" s="5"/>
+      <c r="R371" s="5"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>